<commit_message>
Completed No auth negative cases for batch module
</commit_message>
<xml_diff>
--- a/Team05_APITesters/src/test/resources/Program.xlsx
+++ b/Team05_APITesters/src/test/resources/Program.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\durga\eclipse-workspace\Team05_APITesters\Team05_APITesters\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E5328C3-34C0-48F8-8896-5AA5053DDFAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4B62C56-1C8E-423A-B178-7DBAB9B5E5EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="programController" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="39">
   <si>
     <t>programDescription</t>
   </si>
@@ -114,25 +114,31 @@
     <t>AutomationApiTesting223</t>
   </si>
   <si>
-    <t>Mar24-APITesters-SDET-231</t>
-  </si>
-  <si>
-    <t>Mar24-APITesters-SDET-232</t>
-  </si>
-  <si>
-    <t>Mar24-APITesters-SDET-updated-231</t>
-  </si>
-  <si>
-    <t>Mar24-APITesters-SDET-updatedPgm-231</t>
-  </si>
-  <si>
     <t>For no auth valida data</t>
   </si>
   <si>
     <t>For postive flow</t>
   </si>
   <si>
-    <t>SoftwareTesting231</t>
+    <t>SoftwareTesting246</t>
+  </si>
+  <si>
+    <t>Mar24-APITesters-SDET-246</t>
+  </si>
+  <si>
+    <t>Mar24-APITesters-SDET-247</t>
+  </si>
+  <si>
+    <t>Mar24-APITesters-SDET-updated-246</t>
+  </si>
+  <si>
+    <t>Mar24-APITesters-SDET-updated-247</t>
+  </si>
+  <si>
+    <t>Mar24-APITesters-SDET-updatedPgm-247</t>
+  </si>
+  <si>
+    <t>Mar24-APITesters-SDET-updatedPgm-246</t>
   </si>
 </sst>
 </file>
@@ -503,7 +509,7 @@
         <v>27</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>9</v>
@@ -537,7 +543,7 @@
   <dimension ref="A1:I8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2"/>
@@ -583,7 +589,7 @@
         <v>28</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="C2" t="s">
         <v>9</v>
@@ -592,10 +598,10 @@
         <v>10</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="G2" s="7" t="s">
         <v>9</v>
@@ -604,7 +610,7 @@
         <v>11</v>
       </c>
       <c r="I2" s="7" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -612,7 +618,7 @@
         <v>29</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="C3" t="s">
         <v>9</v>
@@ -621,10 +627,10 @@
         <v>10</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="G3" s="7" t="s">
         <v>9</v>
@@ -633,7 +639,7 @@
         <v>11</v>
       </c>
       <c r="I3" s="7" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
     </row>
     <row r="5" spans="1:9">

</xml_diff>